<commit_message>
not sure what the update was but ill push it anywat bc ermm idk
</commit_message>
<xml_diff>
--- a/main_hw/SUMEC_MK_V/bom/SUMEC_MK_V.xlsx
+++ b/main_hw/SUMEC_MK_V/bom/SUMEC_MK_V.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\Sumec-MiniSumo-HW\main_hw\SUMEC_MK_V\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F142BE73-FE09-4BA7-9BCF-5921C13683FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C86EFBD-21C0-42D6-9B9D-1384F0E9B8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{318D0819-0F8D-4535-926A-50240C04F6C9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="162">
   <si>
     <t>Value</t>
   </si>
@@ -458,6 +458,54 @@
   </si>
   <si>
     <t>24CW1280T-I/OT EEPROM</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>ENOUGH</t>
+  </si>
+  <si>
+    <t>DNB</t>
+  </si>
+  <si>
+    <t>*DNB = DO NOT BUY</t>
+  </si>
+  <si>
+    <t>4+6</t>
+  </si>
+  <si>
+    <t>8+2</t>
+  </si>
+  <si>
+    <t>~60</t>
+  </si>
+  <si>
+    <t>14+4</t>
+  </si>
+  <si>
+    <t>9+2</t>
+  </si>
+  <si>
+    <t>10+5</t>
+  </si>
+  <si>
+    <t>9+4</t>
+  </si>
+  <si>
+    <t>10+10</t>
+  </si>
+  <si>
+    <t>5+1</t>
+  </si>
+  <si>
+    <t>ATtiny85-20S</t>
+  </si>
+  <si>
+    <t>QRE1113GR</t>
+  </si>
+  <si>
+    <t>Molex PicoBlade, 4 Pin, horizontal, mouser</t>
   </si>
 </sst>
 </file>
@@ -608,7 +656,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -815,6 +863,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,7 +1049,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1009,9 +1063,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1021,6 +1072,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % – Zvýraznění 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1397,20 +1458,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C378E24-255E-4758-9EA3-ADC3BD7350B6}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.90625" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="36" style="9" customWidth="1"/>
+    <col min="5" max="5" width="35" style="9" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -1426,699 +1488,865 @@
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>106</v>
       </c>
+      <c r="F1" s="8" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="F2" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="9">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>127</v>
       </c>
+      <c r="F3" s="9" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="9">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>126</v>
       </c>
+      <c r="F4" s="9" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="9">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>125</v>
       </c>
+      <c r="F5" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>124</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>128</v>
       </c>
+      <c r="F7" s="9" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="9">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>129</v>
       </c>
+      <c r="F8" s="9" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="F11" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="F12" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C13" s="9">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="F13" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="F14" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C15" s="9">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="F15" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="F18" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C19" s="9">
         <v>7</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="F19" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C20" s="9">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="F20" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="F22" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C23" s="9">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="F23" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="F25" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="F27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="5">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="F28" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C29" s="9">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="F29" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="5">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C31" s="9">
         <v>5</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="F31" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C32" s="9">
         <v>5</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D32" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="F32" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="5">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="F33" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="5">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="F34" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C35" s="9">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="F35" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="5">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="5">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="5">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E39" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="F39" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="5">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E40" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="F40" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="5">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C41" s="9">
+        <v>1</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>96</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F43" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="9">
+        <v>2</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F45" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1" xr:uid="{AAA11C5E-2BF9-47DA-B820-FAE981004733}"/>
-    <hyperlink ref="E37" r:id="rId2" xr:uid="{6C250A31-FBED-4F67-A89D-CAA523673A12}"/>
-    <hyperlink ref="E30" r:id="rId3" display="0R. 250mW, 0805" xr:uid="{AF1D7AC8-536F-42CC-A74F-EE3422B02B14}"/>
-    <hyperlink ref="E27" r:id="rId4" display="15R mouser" xr:uid="{A8636B5C-1C02-4D4C-8004-E9F78945D9E7}"/>
-    <hyperlink ref="E31" r:id="rId5" display="100R, 250mW, 0805" xr:uid="{B838D7C1-3EA2-4EB4-8DA1-A01E486F7BEF}"/>
-    <hyperlink ref="E21" r:id="rId6" display="10k mouser" xr:uid="{5BFA8E4A-B85F-490A-9C3F-D1AEF83C79A9}"/>
-    <hyperlink ref="E16" r:id="rId7" xr:uid="{AE35E0C0-A83A-4128-99A9-CD65E7C5496E}"/>
-    <hyperlink ref="E17" r:id="rId8" xr:uid="{BA0E193C-E7F6-4B84-9BF6-B61D7B72D1EA}"/>
-    <hyperlink ref="E15" r:id="rId9" xr:uid="{6286FC92-FA1B-442B-BF15-E23089E424DE}"/>
-    <hyperlink ref="E13" r:id="rId10" xr:uid="{97AA37BA-6BD4-44DB-8D62-A0A3B05662EC}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{0D38694C-81FF-4C44-90DD-E5924AE81C27}"/>
-    <hyperlink ref="E10" r:id="rId12" xr:uid="{9F61ECBF-B31A-430C-8D00-083E431970B1}"/>
-    <hyperlink ref="E9" r:id="rId13" display="Polyfuse, Itrip: 500mA, 16V" xr:uid="{7BD1E806-2870-45B7-83F4-221E24568AAA}"/>
-    <hyperlink ref="E18" r:id="rId14" xr:uid="{B47037B1-D7BA-4B99-8127-5B4849A3804C}"/>
-    <hyperlink ref="E20" r:id="rId15" xr:uid="{9309C829-FA8B-4CAE-AAFF-58F5FD6E827A}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{1D011C7D-831F-4C6E-A574-C8DB52301BBE}"/>
+    <hyperlink ref="E16" r:id="rId1" xr:uid="{AAA11C5E-2BF9-47DA-B820-FAE981004733}"/>
+    <hyperlink ref="E39" r:id="rId2" xr:uid="{6C250A31-FBED-4F67-A89D-CAA523673A12}"/>
+    <hyperlink ref="E32" r:id="rId3" display="0R. 250mW, 0805" xr:uid="{AF1D7AC8-536F-42CC-A74F-EE3422B02B14}"/>
+    <hyperlink ref="E29" r:id="rId4" display="15R mouser" xr:uid="{A8636B5C-1C02-4D4C-8004-E9F78945D9E7}"/>
+    <hyperlink ref="E33" r:id="rId5" display="100R, 250mW, 0805" xr:uid="{B838D7C1-3EA2-4EB4-8DA1-A01E486F7BEF}"/>
+    <hyperlink ref="E23" r:id="rId6" display="10k mouser" xr:uid="{5BFA8E4A-B85F-490A-9C3F-D1AEF83C79A9}"/>
+    <hyperlink ref="E18" r:id="rId7" xr:uid="{AE35E0C0-A83A-4128-99A9-CD65E7C5496E}"/>
+    <hyperlink ref="E19" r:id="rId8" xr:uid="{BA0E193C-E7F6-4B84-9BF6-B61D7B72D1EA}"/>
+    <hyperlink ref="E17" r:id="rId9" xr:uid="{6286FC92-FA1B-442B-BF15-E23089E424DE}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{97AA37BA-6BD4-44DB-8D62-A0A3B05662EC}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{0D38694C-81FF-4C44-90DD-E5924AE81C27}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{9F61ECBF-B31A-430C-8D00-083E431970B1}"/>
+    <hyperlink ref="E11" r:id="rId13" display="Polyfuse, Itrip: 500mA, 16V" xr:uid="{7BD1E806-2870-45B7-83F4-221E24568AAA}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{B47037B1-D7BA-4B99-8127-5B4849A3804C}"/>
+    <hyperlink ref="E22" r:id="rId15" xr:uid="{9309C829-FA8B-4CAE-AAFF-58F5FD6E827A}"/>
+    <hyperlink ref="E21" r:id="rId16" xr:uid="{1D011C7D-831F-4C6E-A574-C8DB52301BBE}"/>
     <hyperlink ref="E6" r:id="rId17" display="22nF, 50V, 0805, mouser, X7R" xr:uid="{B9BE4BFA-A7B6-4F9C-9C43-835D2E1EE321}"/>
     <hyperlink ref="E5" r:id="rId18" display="22uF, 0805 " xr:uid="{7E8A634C-4F58-421D-8348-C5E161BC136D}"/>
     <hyperlink ref="E4" r:id="rId19" display="10uF, 16V, 1206, tantal, mouser" xr:uid="{327ADF4D-9ACB-4939-94F4-572E83029D71}"/>
     <hyperlink ref="E3" r:id="rId20" display="100nF, 16V, 0805, ceramic, mouser X7R" xr:uid="{83727A94-99FC-426D-9947-B51741A389EE}"/>
     <hyperlink ref="E7" r:id="rId21" xr:uid="{8CBEE851-66A7-4AB2-8199-7A8FAC17AF58}"/>
-    <hyperlink ref="F10" r:id="rId22" display="Red LED, 20mA 1.9V, 0805, mouser" xr:uid="{683FAE00-17B5-47D5-984F-2406334C16FC}"/>
-    <hyperlink ref="F8" r:id="rId23" display="Yellow LED, 20mA, 1.9V, 0805, mouser" xr:uid="{422C1099-ED63-46AA-9A34-5F153825DEC7}"/>
-    <hyperlink ref="F9" r:id="rId24" display="Green-Yellow LED, 20mA, 1.9V, mouser" xr:uid="{AD8305B2-A478-491A-A1BA-8771E93952AF}"/>
-    <hyperlink ref="E11" r:id="rId25" display="DRV8874.  mouser" xr:uid="{A8148FD5-DB3A-41FA-8530-8EC8DD8B7D6A}"/>
-    <hyperlink ref="E22" r:id="rId26" xr:uid="{3B82CDEA-3DA3-4155-A96E-FE63616AD061}"/>
-    <hyperlink ref="E23" r:id="rId27" display="45.3k, 125mW, vishay" xr:uid="{B9120E7B-E929-409A-87F2-86F162015FEE}"/>
-    <hyperlink ref="E26" r:id="rId28" display="100k, 250mW, 0805" xr:uid="{4AA81697-DBF5-4B57-A84A-95EA0BD792D3}"/>
-    <hyperlink ref="E24" r:id="rId29" display="15k, 125mW, vishay" xr:uid="{838C3CC0-CF6C-4811-B281-A8DC0BD6D6BF}"/>
-    <hyperlink ref="E25" r:id="rId30" xr:uid="{EF6E2CF6-89B0-496F-9D16-FD277AF6483E}"/>
-    <hyperlink ref="E28" r:id="rId31" xr:uid="{7609A1DD-9F3C-4C85-B940-7046AB5B8714}"/>
-    <hyperlink ref="E29" r:id="rId32" display="220R 250mW" xr:uid="{8AAF3261-CF92-4F7C-B4C6-CE4880A149D4}"/>
+    <hyperlink ref="E10" r:id="rId22" display="Red LED, 20mA 1.9V, 0805, mouser" xr:uid="{683FAE00-17B5-47D5-984F-2406334C16FC}"/>
+    <hyperlink ref="E8" r:id="rId23" display="Yellow LED, 20mA, 1.9V, 0805, mouser" xr:uid="{422C1099-ED63-46AA-9A34-5F153825DEC7}"/>
+    <hyperlink ref="E9" r:id="rId24" display="Green-Yellow LED, 20mA, 1.9V, mouser" xr:uid="{AD8305B2-A478-491A-A1BA-8771E93952AF}"/>
+    <hyperlink ref="E13" r:id="rId25" display="DRV8874.  mouser" xr:uid="{A8148FD5-DB3A-41FA-8530-8EC8DD8B7D6A}"/>
+    <hyperlink ref="E24" r:id="rId26" xr:uid="{3B82CDEA-3DA3-4155-A96E-FE63616AD061}"/>
+    <hyperlink ref="E25" r:id="rId27" display="45.3k, 125mW, vishay" xr:uid="{B9120E7B-E929-409A-87F2-86F162015FEE}"/>
+    <hyperlink ref="E28" r:id="rId28" display="100k, 250mW, 0805" xr:uid="{4AA81697-DBF5-4B57-A84A-95EA0BD792D3}"/>
+    <hyperlink ref="E26" r:id="rId29" display="15k, 125mW, vishay" xr:uid="{838C3CC0-CF6C-4811-B281-A8DC0BD6D6BF}"/>
+    <hyperlink ref="E27" r:id="rId30" xr:uid="{EF6E2CF6-89B0-496F-9D16-FD277AF6483E}"/>
+    <hyperlink ref="E30" r:id="rId31" xr:uid="{7609A1DD-9F3C-4C85-B940-7046AB5B8714}"/>
+    <hyperlink ref="E31" r:id="rId32" display="220R 250mW" xr:uid="{8AAF3261-CF92-4F7C-B4C6-CE4880A149D4}"/>
     <hyperlink ref="E2" r:id="rId33" xr:uid="{7F3D7B4D-183A-4801-9525-370FB3F9FAB6}"/>
-    <hyperlink ref="E34" r:id="rId34" display="INA226" xr:uid="{397D6788-B795-41C0-86EF-5D9A672512ED}"/>
-    <hyperlink ref="E32" r:id="rId35" xr:uid="{6ACBACFE-23B3-49C2-90F6-6AA330F8874A}"/>
-    <hyperlink ref="E33" r:id="rId36" xr:uid="{49963810-7914-4564-BFD2-896B31B7F778}"/>
-    <hyperlink ref="E35" r:id="rId37" xr:uid="{A2FBFBCD-8434-46C6-A312-F237777DEFC5}"/>
-    <hyperlink ref="E36" r:id="rId38" display="24CW1280T-I/OT EEPROMe" xr:uid="{A253018A-2864-4CFF-A4DC-9B4C45FEEFBA}"/>
+    <hyperlink ref="E36" r:id="rId34" display="INA226" xr:uid="{397D6788-B795-41C0-86EF-5D9A672512ED}"/>
+    <hyperlink ref="E34" r:id="rId35" xr:uid="{6ACBACFE-23B3-49C2-90F6-6AA330F8874A}"/>
+    <hyperlink ref="E35" r:id="rId36" xr:uid="{49963810-7914-4564-BFD2-896B31B7F778}"/>
+    <hyperlink ref="E37" r:id="rId37" xr:uid="{A2FBFBCD-8434-46C6-A312-F237777DEFC5}"/>
+    <hyperlink ref="E38" r:id="rId38" display="24CW1280T-I/OT EEPROMe" xr:uid="{A253018A-2864-4CFF-A4DC-9B4C45FEEFBA}"/>
+    <hyperlink ref="E43" r:id="rId39" xr:uid="{F2E7DCA4-3390-4425-9B2C-EFCF6D7420A9}"/>
+    <hyperlink ref="E44" r:id="rId40" xr:uid="{A8B3F5AD-ACFD-42FC-BC5B-B8D4D6899151}"/>
+    <hyperlink ref="E45" r:id="rId41" xr:uid="{E08DD23C-5B5C-4170-A93D-CA34B22392B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>